<commit_message>
majority v3.15.4 - Fully automatic installation script ready
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
   <si>
     <t>***** MAJORITY *****</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>*5 - doesn't really mean much (anything?) since we can only get data saying "on/ok" or "error" (see *4) and if more than the threshold% is in error it will go to error anyway, because ERROR state has priority</t>
+  </si>
+  <si>
+    <t>&lt; threshold</t>
   </si>
 </sst>
 </file>
@@ -544,22 +547,10 @@
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -588,6 +579,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -912,944 +915,966 @@
       </c>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18">
+      <c r="C8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
         <v>0.95</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="23" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="29"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="2"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="12">
         <v>0.95</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="25"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="8"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <v>0.05</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="27"/>
+      <c r="E10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="4"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="25"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="18">
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
         <v>0.95</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="23" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="29"/>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="2"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="12">
         <v>0.95</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="25"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="8"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="13">
         <v>0.05</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="27"/>
+      <c r="E14" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="4"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="25"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14">
         <v>0.95</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="29"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="2"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="12">
         <v>0.95</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="25"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="8"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="13">
         <v>0.05</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="27"/>
+      <c r="E18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="4"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="18">
-        <v>1</v>
-      </c>
-      <c r="E20" s="28" t="s">
+      <c r="C20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="23" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="29"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="2"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="16">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24" t="s">
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="25"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="8"/>
-      <c r="C22" s="11" t="s">
+      <c r="B22" s="35"/>
+      <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="13">
         <v>0</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="27"/>
+      <c r="E22" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="4"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="25"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="18">
+      <c r="C24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14">
         <v>0.95</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="35" t="s">
+      <c r="F24" s="19"/>
+      <c r="G24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="29"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="2"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="37"/>
+      <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="12">
         <v>0.05</v>
       </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="25"/>
+      <c r="E25" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="8"/>
-      <c r="C26" s="11" t="s">
+      <c r="B26" s="35"/>
+      <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="27"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="4"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="25"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="14">
         <v>0.95</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="35" t="s">
+      <c r="E28" s="24"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="35" t="s">
+      <c r="I28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="29"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="2"/>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="37"/>
+      <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="12">
         <v>0.05</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="25"/>
+      <c r="E29" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="8"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="35"/>
+      <c r="C30" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="27"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="4"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="25"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="18">
+      <c r="C32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14">
         <v>0.99</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J32" s="29"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="8"/>
-      <c r="C33" s="11" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="13">
         <v>0.01</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="27"/>
+      <c r="E33" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" spans="2:10">
-      <c r="B34" s="4"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="25"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="21"/>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="18">
-        <v>1</v>
-      </c>
-      <c r="E35" s="28" t="s">
+      <c r="C35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J35" s="29"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="8"/>
-      <c r="C36" s="11" t="s">
+      <c r="B36" s="35"/>
+      <c r="C36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="13">
         <v>0</v>
       </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="27"/>
+      <c r="E36" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" spans="2:10">
-      <c r="B37" s="4"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="25"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="21"/>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="18">
-        <v>1</v>
-      </c>
-      <c r="E38" s="28" t="s">
+      <c r="C38" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="14">
+        <v>1</v>
+      </c>
+      <c r="E38" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H38" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="29"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="8"/>
-      <c r="C39" s="11" t="s">
+      <c r="B39" s="35"/>
+      <c r="C39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="13">
         <v>0</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="27"/>
+      <c r="E39" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="23"/>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="4"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="25"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="21"/>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="18">
+      <c r="C41" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="14">
         <v>0.95</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J41" s="29"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="2"/>
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="12">
         <v>0.06</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="25"/>
+      <c r="E42" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="8"/>
-      <c r="C43" s="11" t="s">
+      <c r="B43" s="35"/>
+      <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="13">
         <v>0.4</v>
       </c>
-      <c r="E43" s="26"/>
-      <c r="F43" s="32" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="27"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="4"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="25"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="21"/>
     </row>
     <row r="45" spans="2:10">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="18">
-        <v>1</v>
-      </c>
-      <c r="E45" s="28" t="s">
+      <c r="C45" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H45" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J45" s="29"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="8"/>
-      <c r="C46" s="11" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="13">
         <v>0</v>
       </c>
-      <c r="E46" s="26"/>
-      <c r="F46" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="27"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="23"/>
     </row>
     <row r="47" spans="2:10">
-      <c r="B47" s="4"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="25"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="21"/>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="18">
-        <v>1</v>
-      </c>
-      <c r="E48" s="28" t="s">
+      <c r="C48" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="E48" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J48" s="29"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="25"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="8"/>
-      <c r="C49" s="11" t="s">
+      <c r="B49" s="35"/>
+      <c r="C49" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="13">
         <v>0</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="27"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="23"/>
     </row>
     <row r="50" spans="2:10">
-      <c r="B50" s="4"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="25"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="21"/>
     </row>
     <row r="51" spans="2:10">
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="18">
-        <v>1</v>
-      </c>
-      <c r="E51" s="28" t="s">
+      <c r="C51" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="14">
+        <v>1</v>
+      </c>
+      <c r="E51" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H51" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" s="29"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" s="25"/>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="8"/>
-      <c r="C52" s="11" t="s">
+      <c r="B52" s="35"/>
+      <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="13">
         <v>0</v>
       </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="27"/>
+      <c r="E52" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="23"/>
     </row>
     <row r="53" spans="2:10">
-      <c r="B53" s="4"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="25"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="21"/>
     </row>
     <row r="54" spans="2:10">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="18">
-        <v>1</v>
-      </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H54" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J54" s="29"/>
+      <c r="C54" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="14">
+        <v>1</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="25"/>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="8"/>
-      <c r="C55" s="11" t="s">
+      <c r="B55" s="35"/>
+      <c r="C55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="13">
         <v>0</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="E55" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F55" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="27"/>
+      <c r="F55" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="23"/>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="4"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="25"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="21"/>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="18">
-        <v>1</v>
-      </c>
-      <c r="E57" s="28"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H57" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I57" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J57" s="29"/>
+      <c r="C57" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="14">
+        <v>1</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="25"/>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B58" s="5"/>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="36"/>
+      <c r="C58" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="19">
+      <c r="D58" s="15">
         <v>0</v>
       </c>
-      <c r="E58" s="36" t="s">
+      <c r="E58" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F58" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="30"/>
-      <c r="J58" s="31"/>
+      <c r="F58" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="27"/>
     </row>
     <row r="61" spans="2:10">
       <c r="B61" t="s">
@@ -1878,6 +1903,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B57:B58"/>
@@ -1887,12 +1918,6 @@
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
majority v3.15.21 - add .reserve1 to majority dpConnect list and recreate the majority conf. Policy on the LV and TEMP readings changed - if there's no communication then always report all affected channels as not being on nor in error and do not care about those two in ON, OUTER_ON and STANDBY states (do care only in ERROR).
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="48">
   <si>
     <t>***** MAJORITY *****</t>
   </si>
@@ -150,13 +150,16 @@
     <t>*2 - could require "more than threshold %", but would have to wait for timeout which is quite long (10min?)</t>
   </si>
   <si>
-    <t xml:space="preserve"> &gt; threshold *5</t>
-  </si>
-  <si>
     <t>*5 - doesn't really mean much (anything?) since we can only get data saying "on/ok" or "error" (see *4) and if more than the threshold% is in error it will go to error anyway, because ERROR state has priority</t>
   </si>
   <si>
     <t>&lt; threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *5</t>
+  </si>
+  <si>
+    <t>*5</t>
   </si>
 </sst>
 </file>
@@ -582,13 +585,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -969,7 +972,7 @@
       <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="37"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
@@ -988,7 +991,7 @@
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
@@ -996,7 +999,7 @@
         <v>0.05</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>28</v>
@@ -1043,7 +1046,7 @@
       <c r="J12" s="25"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="37"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1065,7 @@
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>0.05</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>28</v>
@@ -1117,7 +1120,7 @@
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="37"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1139,7 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="35"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>0.05</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>28</v>
@@ -1191,7 +1194,7 @@
       <c r="J20" s="25"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="37"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1210,7 +1213,7 @@
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="35"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>28</v>
@@ -1254,18 +1257,18 @@
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J24" s="25"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="37"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>0.05</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>28</v>
@@ -1284,7 +1287,7 @@
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="35"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
@@ -1326,18 +1329,18 @@
       <c r="E28" s="24"/>
       <c r="F28" s="19"/>
       <c r="G28" s="31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H28" s="31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I28" s="31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="37"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>0.05</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>28</v>
@@ -1356,7 +1359,7 @@
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="35"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="7" t="s">
         <v>4</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="35"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="7" t="s">
         <v>3</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>0.01</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>28</v>
@@ -1466,7 +1469,7 @@
       <c r="J35" s="25"/>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="35"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="7" t="s">
         <v>3</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>28</v>
@@ -1521,7 +1524,7 @@
       <c r="J38" s="25"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="35"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="7" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>28</v>
@@ -1574,7 +1577,7 @@
       <c r="J41" s="25"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="37"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="6" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>0.06</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>28</v>
@@ -1593,7 +1596,7 @@
       <c r="J42" s="21"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="35"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
@@ -1646,7 +1649,7 @@
       <c r="J45" s="25"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="35"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="7" t="s">
         <v>3</v>
       </c>
@@ -1699,7 +1702,7 @@
       <c r="J48" s="25"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="35"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="7" t="s">
         <v>3</v>
       </c>
@@ -1752,7 +1755,7 @@
       <c r="J51" s="25"/>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="35"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>28</v>
@@ -1805,7 +1808,7 @@
       <c r="J54" s="25"/>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="35"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="7" t="s">
         <v>3</v>
       </c>
@@ -1858,7 +1861,7 @@
       <c r="J57" s="25"/>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B58" s="36"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="9" t="s">
         <v>3</v>
       </c>
@@ -1898,17 +1901,11 @@
     </row>
     <row r="65" spans="2:2">
       <c r="B65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B26"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B57:B58"/>
@@ -1918,6 +1915,12 @@
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
majority v3.15.23 - decrease error threshold for HV devices down to 3% to be able to see when a channel trips! enabled all FSM manipulation in setup. gogogo! :)
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -891,7 +891,7 @@
   <dimension ref="B3:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -996,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>45</v>
@@ -1070,7 +1070,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>45</v>
@@ -1144,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
majority v3.15.40 - reconfigure majority fo 97% threshold for HV ON and STANDBY
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -585,13 +585,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -891,7 +891,7 @@
   <dimension ref="B3:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -972,7 +972,7 @@
       <c r="J8" s="25"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="36"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="14">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>26</v>
@@ -1046,12 +1046,12 @@
       <c r="J12" s="25"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="35"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="12">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>26</v>
@@ -1065,7 +1065,7 @@
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="36"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="35"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="36"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="J20" s="25"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="35"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1213,7 @@
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="36"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="J24" s="25"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="35"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="36"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
@@ -1340,7 +1340,7 @@
       <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="35"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="36"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="7" t="s">
         <v>4</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="J32" s="25"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="36"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="7" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1469,7 @@
       <c r="J35" s="25"/>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="36"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="7" t="s">
         <v>3</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="J38" s="25"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="36"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="7" t="s">
         <v>3</v>
       </c>
@@ -1577,7 +1577,7 @@
       <c r="J41" s="25"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="35"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="6" t="s">
         <v>3</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="J42" s="21"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="36"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="7" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="J45" s="25"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="36"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="7" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="J48" s="25"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="36"/>
+      <c r="B49" s="35"/>
       <c r="C49" s="7" t="s">
         <v>3</v>
       </c>
@@ -1755,7 +1755,7 @@
       <c r="J51" s="25"/>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="36"/>
+      <c r="B52" s="35"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="J54" s="25"/>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="36"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="7" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="J57" s="25"/>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B58" s="37"/>
+      <c r="B58" s="36"/>
       <c r="C58" s="9" t="s">
         <v>3</v>
       </c>
@@ -1906,6 +1906,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B57:B58"/>
@@ -1915,12 +1921,6 @@
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DCS UI v3.2.2 - value monitor loading delay decreased to 25s. Access control in Xmas monitoring control panel and Maraton individual channels control panel. Updated documentation (HV_OUTER ON threshold 95% -> 97%)
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -596,10 +596,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -608,8 +607,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,7 +907,7 @@
   <dimension ref="B3:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,7 +930,7 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1">
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="33" t="s">
         <v>34</v>
       </c>
     </row>
@@ -959,19 +959,19 @@
       <c r="I7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="34" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="13">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>26</v>
@@ -989,12 +989,12 @@
       <c r="J8" s="24"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="34"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="11">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>26</v>
@@ -1008,7 +1008,7 @@
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1063,7 +1063,7 @@
       <c r="J12" s="24"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="34"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="J13" s="20"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="6" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1137,7 +1137,7 @@
       <c r="J16" s="24"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="34"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1156,7 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="35"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
@@ -1186,7 +1186,7 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1211,7 +1211,7 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="34"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="35"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1285,7 +1285,7 @@
       <c r="J24" s="24"/>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="34"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="5" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="J25" s="20"/>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="35"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="6" t="s">
         <v>4</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1357,7 +1357,7 @@
       <c r="J28" s="24"/>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="34"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="35"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="6" t="s">
         <v>4</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -1431,7 +1431,7 @@
       <c r="J32" s="24"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="35"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="6" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="2:10">
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -1486,7 +1486,7 @@
       <c r="J35" s="24"/>
     </row>
     <row r="36" spans="2:10">
-      <c r="B36" s="35"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="6" t="s">
         <v>3</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="J37" s="20"/>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1541,7 +1541,7 @@
       <c r="J38" s="24"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="35"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6" t="s">
         <v>3</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="J40" s="20"/>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -1594,7 +1594,7 @@
       <c r="J41" s="24"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="34"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="5" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="J42" s="20"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="35"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6" t="s">
         <v>4</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="J44" s="20"/>
     </row>
     <row r="45" spans="2:10">
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -1666,7 +1666,7 @@
       <c r="J45" s="24"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="35"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="33" t="s">
+      <c r="B48" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -1719,7 +1719,7 @@
       <c r="J48" s="24"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="35"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="6" t="s">
         <v>3</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="2:10">
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -1772,7 +1772,7 @@
       <c r="J51" s="24"/>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" s="35"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="6" t="s">
         <v>3</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="J53" s="20"/>
     </row>
     <row r="54" spans="2:10">
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -1825,7 +1825,7 @@
       <c r="J54" s="24"/>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="35"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="6" t="s">
         <v>3</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="J56" s="20"/>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -1878,7 +1878,7 @@
       <c r="J57" s="24"/>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B58" s="36"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="8" t="s">
         <v>3</v>
       </c>
@@ -1923,6 +1923,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B57:B58"/>
@@ -1932,12 +1938,6 @@
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
majority 5.15.0 - takes into account the on-voltage settings for individual UF/PNPI HV channels - compatible with CMS_CSCfw_HV_CC version 3.1.0
</commit_message>
<xml_diff>
--- a/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
+++ b/EMU/DCS/Majority/CMS_CSC_majority/documentation.xlsx
@@ -49,7 +49,7 @@
     <t>STANDBY (all and'ed)</t>
   </si>
   <si>
-    <t>NOY-READY - everything else (should be a transition)</t>
+    <t>NOY-READY - everything else</t>
   </si>
   <si>
     <t>HV_OUTER</t>
@@ -58,10 +58,10 @@
     <t>on</t>
   </si>
   <si>
-    <t> == 0%</t>
-  </si>
-  <si>
-    <t> &gt; threshold</t>
+    <t>== 0%</t>
+  </si>
+  <si>
+    <t>&gt; threshold</t>
   </si>
   <si>
     <t>standby</t>
@@ -225,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="29">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -384,20 +384,6 @@
       <left style="medium"/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -503,18 +489,18 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="14" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="15" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="16" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="23" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="24" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="19" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="20" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="25" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="23" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="26" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="27" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="28" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="29" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="30" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="24" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="25" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="26" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="27" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="28" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -599,17 +585,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.756862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9137254901961"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.6627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7921568627451"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.7411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9803921568627"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.756862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.878431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.0705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.8" outlineLevel="0" r="3">
@@ -947,7 +933,7 @@
       <c r="I23" s="29"/>
       <c r="J23" s="30"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="B24" s="9" t="s">
         <v>21</v>
       </c>
@@ -1617,7 +1603,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="8" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="8" scale="95" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1637,7 +1623,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1662,7 +1648,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>